<commit_message>
Añadido borrar y crear pelis
</commit_message>
<xml_diff>
--- a/INSERTS.xlsx
+++ b/INSERTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\DAW\M12\netflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9AF666A-C6A7-4714-A703-FDA816F206E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7072B13-C01C-4080-BB92-2C8250000D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="432" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{48DE31D5-4A6D-472A-B5CD-F89AB0710D09}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{48DE31D5-4A6D-472A-B5CD-F89AB0710D09}"/>
   </bookViews>
   <sheets>
     <sheet name="Peliculas" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="reparto_peli" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -776,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285EED17-E58E-4660-BEA3-ABA9746F39A6}">
   <dimension ref="B3:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:F13"/>
     </sheetView>
   </sheetViews>
@@ -1235,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E952BA40-FD13-4629-A8E6-55E9D692CD7E}">
   <dimension ref="B1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:H17"/>
     </sheetView>
   </sheetViews>

</xml_diff>